<commit_message>
extract features from DTE sub-net
</commit_message>
<xml_diff>
--- a/S3/S3.xlsx
+++ b/S3/S3.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>I03_01_1</t>
   </si>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I48" zoomScale="154" workbookViewId="0">
-      <selection activeCell="U63" sqref="U63"/>
+    <sheetView tabSelected="1" topLeftCell="O21" zoomScale="121" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1203,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>17</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>18</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>20</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>21</v>
       </c>
@@ -1301,6 +1301,14 @@
       </c>
       <c r="L38">
         <v>3.16</v>
+      </c>
+      <c r="P38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="T48" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="12:21" x14ac:dyDescent="0.25">

</xml_diff>